<commit_message>
change abs paths to rel paths
</commit_message>
<xml_diff>
--- a/Figure 2 and Figure 3/data_flow/data/final_results.xlsx
+++ b/Figure 2 and Figure 3/data_flow/data/final_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\no-one-is-a-group\Fig5_6\data_flow\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\No-One-is-a-Group-Software-Repository\Figure 2 and Figure 3\data_flow\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3A573C-CDCE-4F49-B35F-4DAB85A8530C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0866E6-D367-416C-9E2A-EFE9A419E345}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A16:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>